<commit_message>
Have done Mtmoproject with excel, package 9
</commit_message>
<xml_diff>
--- a/web/test.xlsx
+++ b/web/test.xlsx
@@ -78,7 +78,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Лікар, що створив взаємодію</t>
@@ -134,8 +134,18 @@
           <t>9.10</t>
         </is>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Всього</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Гаврилюк Світлана Володимирівна</t>
@@ -156,8 +166,14 @@
       <c r="K2" s="0">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="0">
+        <v>747</v>
+      </c>
+      <c r="M2" s="0">
+        <v>37.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="0" t="inlineStr">
         <is>
           <t>Глушко Наталія Григорівна</t>
@@ -169,8 +185,14 @@
       <c r="F3" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="0">
+        <v>882</v>
+      </c>
+      <c r="M3" s="0">
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="0" t="inlineStr">
         <is>
           <t>Рибак Тетяна Миколаївна</t>
@@ -179,8 +201,14 @@
       <c r="K4" s="0">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="0">
+        <v>3132</v>
+      </c>
+      <c r="M4" s="0">
+        <v>156.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="0" t="inlineStr">
         <is>
           <t>Кащенюк Олексій Леонідович</t>
@@ -189,8 +217,14 @@
       <c r="H5" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="0">
+        <v>3195</v>
+      </c>
+      <c r="M5" s="0">
+        <v>159.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="0" t="inlineStr">
         <is>
           <t>Пінчук Олексій Миколайович</t>
@@ -199,8 +233,14 @@
       <c r="K6" s="0">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="0">
+        <v>4185</v>
+      </c>
+      <c r="M6" s="0">
+        <v>209.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="0" t="inlineStr">
         <is>
           <t>Хомич Олег Андрійович</t>
@@ -215,8 +255,14 @@
       <c r="K7" s="0">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="0">
+        <v>4455</v>
+      </c>
+      <c r="M7" s="0">
+        <v>222.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="0" t="inlineStr">
         <is>
           <t>Карпюк Лариса Іванівна</t>
@@ -225,8 +271,14 @@
       <c r="D8" s="0">
         <v>369</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="0">
+        <v>5562</v>
+      </c>
+      <c r="M8" s="0">
+        <v>278.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="0" t="inlineStr">
         <is>
           <t>Третяк Ірина Борисівна</t>
@@ -235,8 +287,14 @@
       <c r="H9" s="0">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="0">
+        <v>5688</v>
+      </c>
+      <c r="M9" s="0">
+        <v>284.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="0" t="inlineStr">
         <is>
           <t>Березюк Світлана Вікторівна</t>
@@ -245,8 +303,14 @@
       <c r="D10" s="0">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="0">
+        <v>5985</v>
+      </c>
+      <c r="M10" s="0">
+        <v>299.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="0" t="inlineStr">
         <is>
           <t>Рудь Юрій Євгенович</t>
@@ -264,8 +328,14 @@
       <c r="J11" s="0">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="0">
+        <v>7731</v>
+      </c>
+      <c r="M11" s="0">
+        <v>386.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="0" t="inlineStr">
         <is>
           <t>Жук Тетяна Йосипівна</t>
@@ -286,8 +356,14 @@
       <c r="K12" s="0">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="0">
+        <v>11124</v>
+      </c>
+      <c r="M12" s="0">
+        <v>556.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="0" t="inlineStr">
         <is>
           <t>Кікавська Тетяна Анатоліївна</t>
@@ -296,8 +372,14 @@
       <c r="F13" s="0">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="0">
+        <v>11349</v>
+      </c>
+      <c r="M13" s="0">
+        <v>567.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="0" t="inlineStr">
         <is>
           <t>Крук Людмила Василівна</t>
@@ -312,8 +394,14 @@
       <c r="K14" s="0">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="0">
+        <v>11889</v>
+      </c>
+      <c r="M14" s="0">
+        <v>594.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="0" t="inlineStr">
         <is>
           <t>Сеник Василь Васильович</t>
@@ -331,8 +419,14 @@
       <c r="K15" s="0">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="0">
+        <v>12879</v>
+      </c>
+      <c r="M15" s="0">
+        <v>643.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="0" t="inlineStr">
         <is>
           <t>Волинюк Уляна Василівна</t>
@@ -347,8 +441,14 @@
       <c r="K16" s="0">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="0">
+        <v>13410</v>
+      </c>
+      <c r="M16" s="0">
+        <v>670.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="0" t="inlineStr">
         <is>
           <t>Байчук Тетяна Микитівна</t>
@@ -363,8 +463,14 @@
       <c r="K17" s="0">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="0">
+        <v>14130</v>
+      </c>
+      <c r="M17" s="0">
+        <v>706.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="0" t="inlineStr">
         <is>
           <t>Сокоринський Валерій Михайлович</t>
@@ -373,8 +479,14 @@
       <c r="B18" s="0">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="0">
+        <v>14238</v>
+      </c>
+      <c r="M18" s="0">
+        <v>711.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="0" t="inlineStr">
         <is>
           <t>Біліч Людмила Степанівна</t>
@@ -383,8 +495,14 @@
       <c r="E19" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="0">
+        <v>14274</v>
+      </c>
+      <c r="M19" s="0">
+        <v>713.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="0" t="inlineStr">
         <is>
           <t>Шабанова Оксана Василівна</t>
@@ -393,8 +511,14 @@
       <c r="C20" s="0">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="0">
+        <v>14355</v>
+      </c>
+      <c r="M20" s="0">
+        <v>717.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="0" t="inlineStr">
         <is>
           <t>Ковальчук Алла Павлівна</t>
@@ -403,8 +527,14 @@
       <c r="D21" s="0">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="0">
+        <v>14409</v>
+      </c>
+      <c r="M21" s="0">
+        <v>720.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="0" t="inlineStr">
         <is>
           <t>Березнюк Ірина Олегівна</t>
@@ -422,8 +552,14 @@
       <c r="K22" s="0">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="0">
+        <v>15021</v>
+      </c>
+      <c r="M22" s="0">
+        <v>751.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="0" t="inlineStr">
         <is>
           <t>Шуляр Юлія Сергіївна</t>
@@ -432,8 +568,14 @@
       <c r="F23" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="0">
+        <v>15066</v>
+      </c>
+      <c r="M23" s="0">
+        <v>753.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="0" t="inlineStr">
         <is>
           <t>Михальчук Олена Володимирівна</t>
@@ -451,8 +593,14 @@
       <c r="K24" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" s="0">
+        <v>15291</v>
+      </c>
+      <c r="M24" s="0">
+        <v>764.55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="0" t="inlineStr">
         <is>
           <t>Іванюк Світлана Петрівна</t>
@@ -461,8 +609,14 @@
       <c r="F25" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="0">
+        <v>15336</v>
+      </c>
+      <c r="M25" s="0">
+        <v>766.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="0" t="inlineStr">
         <is>
           <t>Зайцев Андрій Олександрович</t>
@@ -471,8 +625,14 @@
       <c r="G26" s="0">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="0">
+        <v>15444</v>
+      </c>
+      <c r="M26" s="0">
+        <v>772.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="0" t="inlineStr">
         <is>
           <t>Дмитрук Тетяна Сергіївна</t>
@@ -480,6 +640,12 @@
       </c>
       <c r="H27" s="0">
         <v>9</v>
+      </c>
+      <c r="L27" s="0">
+        <v>15507</v>
+      </c>
+      <c r="M27" s="0">
+        <v>775.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>